<commit_message>
added all dummy data
</commit_message>
<xml_diff>
--- a/Docs.xlsx
+++ b/Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\bankv2\back\Bankv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43128BBE-D990-4831-A92A-73F1BB8BE008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF1B806-E44C-4221-8259-4FE9CF22A627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18495" yWindow="3135" windowWidth="17655" windowHeight="9915" activeTab="2" xr2:uid="{0C4655BD-FD57-4FCB-842E-89F6E826D1F5}"/>
+    <workbookView xWindow="-18450" yWindow="3150" windowWidth="17655" windowHeight="9915" xr2:uid="{0C4655BD-FD57-4FCB-842E-89F6E826D1F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -35,35 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={047DF704-87D3-4D62-AD11-9DB6A7C05150}</author>
-    <author>tc={2EB977B8-61DD-4D1E-80B5-9132EC4416DE}</author>
-  </authors>
-  <commentList>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{047DF704-87D3-4D62-AD11-9DB6A7C05150}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    path parameters?</t>
-      </text>
-    </comment>
-    <comment ref="D9" authorId="1" shapeId="0" xr:uid="{2EB977B8-61DD-4D1E-80B5-9132EC4416DE}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    don't think i need this....</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="86">
   <si>
     <t>type</t>
   </si>
@@ -288,12 +261,6 @@
   </si>
   <si>
     <t>get all employees</t>
-  </si>
-  <si>
-    <t>get an employees customers</t>
-  </si>
-  <si>
-    <t>/user/{name}</t>
   </si>
   <si>
     <t>/account</t>
@@ -333,7 +300,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,14 +308,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,18 +328,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -507,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -524,21 +473,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -550,20 +490,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -581,9 +507,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Escoto Pineda, Brenda (Student)" id="{18CB8FF5-9DF9-4CA7-93E1-0055996D41C4}" userId="S::escot105@mail.chapman.edu::326d8cae-aba0-43f5-8cb3-97257189f6b7" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -881,23 +805,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D7" dT="2020-10-27T17:44:08.43" personId="{18CB8FF5-9DF9-4CA7-93E1-0055996D41C4}" id="{047DF704-87D3-4D62-AD11-9DB6A7C05150}">
-    <text>path parameters?</text>
-  </threadedComment>
-  <threadedComment ref="D9" dT="2020-10-27T20:29:18.75" personId="{18CB8FF5-9DF9-4CA7-93E1-0055996D41C4}" id="{2EB977B8-61DD-4D1E-80B5-9132EC4416DE}">
-    <text>don't think i need this....</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A55677-7B87-4626-9C4F-ACBB09BA78F6}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,11 +1210,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C999A1-6FDD-4C46-8BCB-4130DD249C10}">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C999A1-6FDD-4C46-8BCB-4130DD249C10}">
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,189 +1239,175 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="16" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="16" t="s">
         <v>71</v>
       </c>
+      <c r="C7" s="16"/>
       <c r="D7" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="16" t="s">
         <v>72</v>
       </c>
+      <c r="C8" s="16"/>
       <c r="D8" s="16" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C13" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D14" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>85</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B50">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="/user">
-      <formula>NOT(ISERROR(SEARCH("/user",B1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="/account">
-      <formula>NOT(ISERROR(SEARCH("/account",B1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed account creation issue
</commit_message>
<xml_diff>
--- a/Docs.xlsx
+++ b/Docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\bankv2\back\Bankv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF1B806-E44C-4221-8259-4FE9CF22A627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260C0FAC-9C66-4850-9660-884AAA7ADC91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18450" yWindow="3150" windowWidth="17655" windowHeight="9915" xr2:uid="{0C4655BD-FD57-4FCB-842E-89F6E826D1F5}"/>
+    <workbookView xWindow="-18450" yWindow="3150" windowWidth="17655" windowHeight="9915" activeTab="2" xr2:uid="{0C4655BD-FD57-4FCB-842E-89F6E826D1F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -275,9 +275,6 @@
     <t>get a user's accounts</t>
   </si>
   <si>
-    <t>account object</t>
-  </si>
-  <si>
     <t>add new account</t>
   </si>
   <si>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>/user/info</t>
+  </si>
+  <si>
+    <t>new account object</t>
   </si>
 </sst>
 </file>
@@ -478,22 +478,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -504,10 +489,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -809,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A55677-7B87-4626-9C4F-ACBB09BA78F6}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1213,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C999A1-6FDD-4C46-8BCB-4130DD249C10}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1314,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16" t="s">
@@ -1345,7 +1326,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>65</v>
@@ -1386,10 +1367,10 @@
         <v>75</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1397,13 +1378,13 @@
         <v>59</v>
       </c>
       <c r="B14" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="D14" s="16" t="s">
         <v>82</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>